<commit_message>
accept EXEL in input
</commit_message>
<xml_diff>
--- a/uploads/pollution.xlsx
+++ b/uploads/pollution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Game_Git\ECO\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D68AB4-AFFE-4B9B-831B-619AEEA4C0AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D639779A-F92D-41ED-88D2-945D897DAAD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DF2FA2EE-2C41-485B-9B89-E31D30C8D0DA}"/>
   </bookViews>
@@ -384,15 +384,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0B1B899-9603-4140-B4BC-126F544BCA01}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="B1">
         <v>2</v>
@@ -406,7 +404,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="B2">
         <v>2</v>

</xml_diff>

<commit_message>
done loader and select
</commit_message>
<xml_diff>
--- a/uploads/pollution.xlsx
+++ b/uploads/pollution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Game_Git\ECO\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D639779A-F92D-41ED-88D2-945D897DAAD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA79332A-1A59-496B-84BA-AD4521F5DDE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DF2FA2EE-2C41-485B-9B89-E31D30C8D0DA}"/>
   </bookViews>
@@ -33,6 +33,10 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,52 +386,670 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0B1B899-9603-4140-B4BC-126F544BCA01}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D47"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="B1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1">
-        <v>234.6</v>
+        <v>13647.6</v>
       </c>
       <c r="D1">
-        <v>2034</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>102</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
       <c r="C2">
-        <v>2894.6</v>
+        <v>9064.7999999999993</v>
       </c>
       <c r="D2">
-        <v>2024</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>4.5999999999999996</v>
+        <v>920.52</v>
       </c>
       <c r="D3">
-        <v>2034</v>
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>77292</v>
+      </c>
+      <c r="D4">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>57348</v>
+      </c>
+      <c r="D5">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>14158.8</v>
+      </c>
+      <c r="D6">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>28407.599999999999</v>
+      </c>
+      <c r="D7">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>65916</v>
+      </c>
+      <c r="D8">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>4960.8</v>
+      </c>
+      <c r="D9">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>36648</v>
+      </c>
+      <c r="D10">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>65844</v>
+      </c>
+      <c r="D11">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>8035.2</v>
+      </c>
+      <c r="D12">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>37728</v>
+      </c>
+      <c r="D13">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>72684</v>
+      </c>
+      <c r="D14">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>46152</v>
+      </c>
+      <c r="D15">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>11725</v>
+      </c>
+      <c r="D16">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>17039.2</v>
+      </c>
+      <c r="D17">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>69112</v>
+      </c>
+      <c r="D18">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>7412.4</v>
+      </c>
+      <c r="D19">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>14527.16</v>
+      </c>
+      <c r="D20">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <v>9</v>
+      </c>
+      <c r="C21">
+        <v>17978.939999999999</v>
+      </c>
+      <c r="D21">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>45004.32</v>
+      </c>
+      <c r="D22">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1124557.2</v>
+      </c>
+      <c r="D23">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>1657414.8</v>
+      </c>
+      <c r="D24">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <v>542865.6</v>
+      </c>
+      <c r="D25">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>6</v>
+      </c>
+      <c r="C26">
+        <v>739076.4</v>
+      </c>
+      <c r="D26">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>141983.28</v>
+      </c>
+      <c r="D27">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28">
+        <v>9</v>
+      </c>
+      <c r="C28">
+        <v>19678.716</v>
+      </c>
+      <c r="D28">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <v>7</v>
+      </c>
+      <c r="C29">
+        <v>46265.04</v>
+      </c>
+      <c r="D29">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>148714.20000000001</v>
+      </c>
+      <c r="D30">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31">
+        <v>9</v>
+      </c>
+      <c r="C31">
+        <v>19305.684000000001</v>
+      </c>
+      <c r="D31">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32">
+        <v>7</v>
+      </c>
+      <c r="C32">
+        <v>45862.2</v>
+      </c>
+      <c r="D32">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>601614</v>
+      </c>
+      <c r="D33">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34">
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>773766</v>
+      </c>
+      <c r="D34">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>3</v>
+      </c>
+      <c r="B35">
+        <v>8</v>
+      </c>
+      <c r="C35">
+        <v>857221.2</v>
+      </c>
+      <c r="D35">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>3</v>
+      </c>
+      <c r="B36">
+        <v>8</v>
+      </c>
+      <c r="C36">
+        <v>229779</v>
+      </c>
+      <c r="D36">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>3</v>
+      </c>
+      <c r="B37">
+        <v>8</v>
+      </c>
+      <c r="C37">
+        <v>889740</v>
+      </c>
+      <c r="D37">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>4</v>
+      </c>
+      <c r="B38">
+        <v>8</v>
+      </c>
+      <c r="C38">
+        <v>72766.8</v>
+      </c>
+      <c r="D38">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>4</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39">
+        <v>13195.584000000001</v>
+      </c>
+      <c r="D39">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40">
+        <v>8</v>
+      </c>
+      <c r="C40">
+        <v>70803.360000000001</v>
+      </c>
+      <c r="D40">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>4</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <v>15008.291999999999</v>
+      </c>
+      <c r="D41">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>4</v>
+      </c>
+      <c r="B42">
+        <v>8</v>
+      </c>
+      <c r="C42">
+        <v>74240.639999999999</v>
+      </c>
+      <c r="D42">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>4</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="C43">
+        <v>15697.332</v>
+      </c>
+      <c r="D43">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>4</v>
+      </c>
+      <c r="B44">
+        <v>8</v>
+      </c>
+      <c r="C44">
+        <v>65093.7</v>
+      </c>
+      <c r="D44">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>4</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45">
+        <v>12280.68</v>
+      </c>
+      <c r="D45">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>4</v>
+      </c>
+      <c r="B46">
+        <v>8</v>
+      </c>
+      <c r="C46">
+        <v>70815.960000000006</v>
+      </c>
+      <c r="D46">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>4</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="C47">
+        <v>14780.16</v>
+      </c>
+      <c r="D47">
+        <v>2017</v>
       </c>
     </row>
   </sheetData>

</xml_diff>